<commit_message>
Material list FLM_06 Fix
</commit_message>
<xml_diff>
--- a/downloads/trlist.xlsx
+++ b/downloads/trlist.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cakmur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\cmdocs\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="5" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="ARS" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5804" uniqueCount="1931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5804" uniqueCount="1932">
   <si>
     <t>NO</t>
   </si>
@@ -8191,6 +8191,9 @@
   <si>
     <t>Toplumsal Cinsiyet Eşitliği Ulusal Eylem Planı eğitim, ekonomi, yoksulluk, yetki ve karar alma sürecine katılım, sağlık, medya, çevre ve kurumsal mekanizmalar konularını kapsamaktadır. Bu alanların her biri için mevcut durumu toplumsal cinsiyet eşitliği açısından tanımlayan, toplumsal cinsiyet eşitliğine ulaşılmasının önündeki engelleri analiz eden ayrıca amaçlar,
 hedefler ve somut uygulama stratejilerine yer veren kapsamlı politika dokümanları hazırlanmıştır.</t>
+  </si>
+  <si>
+    <t>Sabancı Vakfı</t>
   </si>
 </sst>
 </file>
@@ -8439,15 +8442,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8457,6 +8451,15 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8675,7 +8678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -8703,22 +8706,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -9383,22 +9386,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -16043,32 +16046,32 @@
       <c r="O203" s="7"/>
     </row>
     <row r="204" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="22" t="s">
+      <c r="A204" s="19" t="s">
         <v>1701</v>
       </c>
-      <c r="B204" s="21" t="s">
+      <c r="B204" s="18" t="s">
         <v>1702</v>
       </c>
-      <c r="C204" s="21" t="s">
+      <c r="C204" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D204" s="21">
+      <c r="D204" s="18">
         <v>2014</v>
       </c>
-      <c r="E204" s="21" t="s">
+      <c r="E204" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F204" s="21" t="s">
+      <c r="F204" s="18" t="s">
         <v>1703</v>
       </c>
-      <c r="G204" s="21" t="s">
+      <c r="G204" s="18" t="s">
         <v>1704</v>
       </c>
-      <c r="H204" s="21" t="s">
+      <c r="H204" s="18" t="s">
         <v>1705</v>
       </c>
-      <c r="I204" s="19"/>
-      <c r="J204" s="20"/>
+      <c r="I204" s="16"/>
+      <c r="J204" s="17"/>
       <c r="K204" s="7"/>
       <c r="L204" s="7"/>
       <c r="M204" s="7"/>
@@ -16076,32 +16079,32 @@
       <c r="O204" s="7"/>
     </row>
     <row r="205" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="22" t="s">
+      <c r="A205" s="19" t="s">
         <v>1706</v>
       </c>
-      <c r="B205" s="21" t="s">
+      <c r="B205" s="18" t="s">
         <v>1707</v>
       </c>
-      <c r="C205" s="21" t="s">
+      <c r="C205" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D205" s="21">
+      <c r="D205" s="18">
         <v>2018</v>
       </c>
-      <c r="E205" s="21" t="s">
+      <c r="E205" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F205" s="21" t="s">
+      <c r="F205" s="18" t="s">
         <v>1708</v>
       </c>
-      <c r="G205" s="21" t="s">
+      <c r="G205" s="18" t="s">
         <v>604</v>
       </c>
-      <c r="H205" s="21" t="s">
+      <c r="H205" s="18" t="s">
         <v>1709</v>
       </c>
-      <c r="I205" s="19"/>
-      <c r="J205" s="20"/>
+      <c r="I205" s="16"/>
+      <c r="J205" s="17"/>
       <c r="K205" s="7"/>
       <c r="L205" s="7"/>
       <c r="M205" s="7"/>
@@ -16109,32 +16112,32 @@
       <c r="O205" s="7"/>
     </row>
     <row r="206" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="22" t="s">
+      <c r="A206" s="19" t="s">
         <v>1710</v>
       </c>
-      <c r="B206" s="21" t="s">
+      <c r="B206" s="18" t="s">
         <v>1711</v>
       </c>
-      <c r="C206" s="21" t="s">
+      <c r="C206" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D206" s="21">
+      <c r="D206" s="18">
         <v>2018</v>
       </c>
-      <c r="E206" s="21" t="s">
+      <c r="E206" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F206" s="21" t="s">
+      <c r="F206" s="18" t="s">
         <v>1712</v>
       </c>
-      <c r="G206" s="21" t="s">
+      <c r="G206" s="18" t="s">
         <v>1713</v>
       </c>
-      <c r="H206" s="21" t="s">
+      <c r="H206" s="18" t="s">
         <v>1714</v>
       </c>
-      <c r="I206" s="19"/>
-      <c r="J206" s="20"/>
+      <c r="I206" s="16"/>
+      <c r="J206" s="17"/>
       <c r="K206" s="7"/>
       <c r="L206" s="7"/>
       <c r="M206" s="7"/>
@@ -16142,32 +16145,32 @@
       <c r="O206" s="7"/>
     </row>
     <row r="207" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="22" t="s">
+      <c r="A207" s="19" t="s">
         <v>1715</v>
       </c>
-      <c r="B207" s="21" t="s">
+      <c r="B207" s="18" t="s">
         <v>1716</v>
       </c>
-      <c r="C207" s="21" t="s">
+      <c r="C207" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D207" s="21">
+      <c r="D207" s="18">
         <v>2018</v>
       </c>
-      <c r="E207" s="21" t="s">
+      <c r="E207" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F207" s="21" t="s">
+      <c r="F207" s="18" t="s">
         <v>1717</v>
       </c>
-      <c r="G207" s="21" t="s">
+      <c r="G207" s="18" t="s">
         <v>1718</v>
       </c>
-      <c r="H207" s="21" t="s">
+      <c r="H207" s="18" t="s">
         <v>1719</v>
       </c>
-      <c r="I207" s="19"/>
-      <c r="J207" s="20"/>
+      <c r="I207" s="16"/>
+      <c r="J207" s="17"/>
       <c r="K207" s="7"/>
       <c r="L207" s="7"/>
       <c r="M207" s="7"/>
@@ -16175,32 +16178,32 @@
       <c r="O207" s="7"/>
     </row>
     <row r="208" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="22" t="s">
+      <c r="A208" s="19" t="s">
         <v>1720</v>
       </c>
-      <c r="B208" s="21" t="s">
+      <c r="B208" s="18" t="s">
         <v>1721</v>
       </c>
-      <c r="C208" s="21" t="s">
+      <c r="C208" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D208" s="21">
+      <c r="D208" s="18">
         <v>2018</v>
       </c>
-      <c r="E208" s="21" t="s">
+      <c r="E208" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F208" s="21" t="s">
+      <c r="F208" s="18" t="s">
         <v>1722</v>
       </c>
-      <c r="G208" s="21" t="s">
+      <c r="G208" s="18" t="s">
         <v>1723</v>
       </c>
-      <c r="H208" s="21" t="s">
+      <c r="H208" s="18" t="s">
         <v>1724</v>
       </c>
-      <c r="I208" s="19"/>
-      <c r="J208" s="20"/>
+      <c r="I208" s="16"/>
+      <c r="J208" s="17"/>
       <c r="K208" s="7"/>
       <c r="L208" s="7"/>
       <c r="M208" s="7"/>
@@ -16208,32 +16211,32 @@
       <c r="O208" s="7"/>
     </row>
     <row r="209" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="22" t="s">
+      <c r="A209" s="19" t="s">
         <v>1725</v>
       </c>
-      <c r="B209" s="21" t="s">
+      <c r="B209" s="18" t="s">
         <v>1726</v>
       </c>
-      <c r="C209" s="21" t="s">
+      <c r="C209" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D209" s="21">
+      <c r="D209" s="18">
         <v>2018</v>
       </c>
-      <c r="E209" s="21" t="s">
+      <c r="E209" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F209" s="21" t="s">
+      <c r="F209" s="18" t="s">
         <v>1727</v>
       </c>
-      <c r="G209" s="21" t="s">
+      <c r="G209" s="18" t="s">
         <v>1728</v>
       </c>
-      <c r="H209" s="21" t="s">
+      <c r="H209" s="18" t="s">
         <v>1729</v>
       </c>
-      <c r="I209" s="19"/>
-      <c r="J209" s="20"/>
+      <c r="I209" s="16"/>
+      <c r="J209" s="17"/>
       <c r="K209" s="7"/>
       <c r="L209" s="7"/>
       <c r="M209" s="7"/>
@@ -16241,32 +16244,32 @@
       <c r="O209" s="7"/>
     </row>
     <row r="210" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="22" t="s">
+      <c r="A210" s="19" t="s">
         <v>1730</v>
       </c>
-      <c r="B210" s="21" t="s">
+      <c r="B210" s="18" t="s">
         <v>1731</v>
       </c>
-      <c r="C210" s="21" t="s">
+      <c r="C210" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D210" s="21">
+      <c r="D210" s="18">
         <v>2018</v>
       </c>
-      <c r="E210" s="21" t="s">
+      <c r="E210" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F210" s="21" t="s">
+      <c r="F210" s="18" t="s">
         <v>1732</v>
       </c>
-      <c r="G210" s="21" t="s">
+      <c r="G210" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="H210" s="21" t="s">
+      <c r="H210" s="18" t="s">
         <v>1733</v>
       </c>
-      <c r="I210" s="19"/>
-      <c r="J210" s="20"/>
+      <c r="I210" s="16"/>
+      <c r="J210" s="17"/>
       <c r="K210" s="7"/>
       <c r="L210" s="7"/>
       <c r="M210" s="7"/>
@@ -16274,28 +16277,28 @@
       <c r="O210" s="7"/>
     </row>
     <row r="211" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="22" t="s">
+      <c r="A211" s="19" t="s">
         <v>1734</v>
       </c>
-      <c r="B211" s="21" t="s">
+      <c r="B211" s="18" t="s">
         <v>1735</v>
       </c>
-      <c r="C211" s="21" t="s">
+      <c r="C211" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D211" s="21">
+      <c r="D211" s="18">
         <v>2011</v>
       </c>
-      <c r="E211" s="21" t="s">
+      <c r="E211" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F211" s="21" t="s">
+      <c r="F211" s="18" t="s">
         <v>1736</v>
       </c>
-      <c r="G211" s="21" t="s">
+      <c r="G211" s="18" t="s">
         <v>1737</v>
       </c>
-      <c r="H211" s="21" t="s">
+      <c r="H211" s="18" t="s">
         <v>1738</v>
       </c>
       <c r="I211" s="7"/>
@@ -16307,28 +16310,28 @@
       <c r="O211" s="7"/>
     </row>
     <row r="212" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="22" t="s">
+      <c r="A212" s="19" t="s">
         <v>1739</v>
       </c>
-      <c r="B212" s="21" t="s">
+      <c r="B212" s="18" t="s">
         <v>1740</v>
       </c>
-      <c r="C212" s="21" t="s">
+      <c r="C212" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D212" s="21">
+      <c r="D212" s="18">
         <v>2015</v>
       </c>
-      <c r="E212" s="21" t="s">
+      <c r="E212" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F212" s="21" t="s">
+      <c r="F212" s="18" t="s">
         <v>1741</v>
       </c>
-      <c r="G212" s="21" t="s">
+      <c r="G212" s="18" t="s">
         <v>1742</v>
       </c>
-      <c r="H212" s="21" t="s">
+      <c r="H212" s="18" t="s">
         <v>1743</v>
       </c>
       <c r="I212" s="7"/>
@@ -16340,28 +16343,28 @@
       <c r="O212" s="7"/>
     </row>
     <row r="213" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="22" t="s">
+      <c r="A213" s="19" t="s">
         <v>1744</v>
       </c>
-      <c r="B213" s="21" t="s">
+      <c r="B213" s="18" t="s">
         <v>1745</v>
       </c>
-      <c r="C213" s="21" t="s">
+      <c r="C213" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D213" s="21">
+      <c r="D213" s="18">
         <v>2018</v>
       </c>
-      <c r="E213" s="21" t="s">
+      <c r="E213" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F213" s="21" t="s">
+      <c r="F213" s="18" t="s">
         <v>1746</v>
       </c>
-      <c r="G213" s="21" t="s">
+      <c r="G213" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="H213" s="21" t="s">
+      <c r="H213" s="18" t="s">
         <v>1747</v>
       </c>
       <c r="I213" s="7"/>
@@ -16373,28 +16376,28 @@
       <c r="O213" s="7"/>
     </row>
     <row r="214" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="22" t="s">
+      <c r="A214" s="19" t="s">
         <v>1748</v>
       </c>
-      <c r="B214" s="21" t="s">
+      <c r="B214" s="18" t="s">
         <v>1749</v>
       </c>
-      <c r="C214" s="21" t="s">
+      <c r="C214" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D214" s="21">
+      <c r="D214" s="18">
         <v>2015</v>
       </c>
-      <c r="E214" s="21" t="s">
+      <c r="E214" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F214" s="21" t="s">
+      <c r="F214" s="18" t="s">
         <v>1750</v>
       </c>
-      <c r="G214" s="21" t="s">
+      <c r="G214" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="H214" s="21" t="s">
+      <c r="H214" s="18" t="s">
         <v>1751</v>
       </c>
       <c r="I214" s="7"/>
@@ -16406,28 +16409,28 @@
       <c r="O214" s="7"/>
     </row>
     <row r="215" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="22" t="s">
+      <c r="A215" s="19" t="s">
         <v>1752</v>
       </c>
-      <c r="B215" s="21" t="s">
+      <c r="B215" s="18" t="s">
         <v>1753</v>
       </c>
-      <c r="C215" s="21" t="s">
+      <c r="C215" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D215" s="21">
+      <c r="D215" s="18">
         <v>2018</v>
       </c>
-      <c r="E215" s="21" t="s">
+      <c r="E215" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F215" s="21" t="s">
+      <c r="F215" s="18" t="s">
         <v>1754</v>
       </c>
-      <c r="G215" s="21" t="s">
+      <c r="G215" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="H215" s="21" t="s">
+      <c r="H215" s="18" t="s">
         <v>1755</v>
       </c>
       <c r="I215" s="7"/>
@@ -16439,28 +16442,28 @@
       <c r="O215" s="7"/>
     </row>
     <row r="216" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="22" t="s">
+      <c r="A216" s="19" t="s">
         <v>1756</v>
       </c>
-      <c r="B216" s="21" t="s">
+      <c r="B216" s="18" t="s">
         <v>1757</v>
       </c>
-      <c r="C216" s="21" t="s">
+      <c r="C216" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D216" s="21">
+      <c r="D216" s="18">
         <v>2018</v>
       </c>
-      <c r="E216" s="21" t="s">
+      <c r="E216" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F216" s="21" t="s">
+      <c r="F216" s="18" t="s">
         <v>1758</v>
       </c>
-      <c r="G216" s="21" t="s">
+      <c r="G216" s="18" t="s">
         <v>1759</v>
       </c>
-      <c r="H216" s="21" t="s">
+      <c r="H216" s="18" t="s">
         <v>1760</v>
       </c>
       <c r="I216" s="7"/>
@@ -16472,158 +16475,158 @@
       <c r="O216" s="7"/>
     </row>
     <row r="217" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="22" t="s">
+      <c r="A217" s="19" t="s">
         <v>1761</v>
       </c>
-      <c r="B217" s="21" t="s">
+      <c r="B217" s="18" t="s">
         <v>1762</v>
       </c>
-      <c r="C217" s="21" t="s">
+      <c r="C217" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D217" s="21">
+      <c r="D217" s="18">
         <v>2010</v>
       </c>
-      <c r="E217" s="21" t="s">
+      <c r="E217" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F217" s="21" t="s">
+      <c r="F217" s="18" t="s">
         <v>1763</v>
       </c>
-      <c r="G217" s="21" t="s">
+      <c r="G217" s="18" t="s">
         <v>1645</v>
       </c>
-      <c r="H217" s="21" t="s">
+      <c r="H217" s="18" t="s">
         <v>1764</v>
       </c>
     </row>
     <row r="218" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="22" t="s">
+      <c r="A218" s="19" t="s">
         <v>1765</v>
       </c>
-      <c r="B218" s="21" t="s">
+      <c r="B218" s="18" t="s">
         <v>1766</v>
       </c>
-      <c r="C218" s="21" t="s">
+      <c r="C218" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D218" s="21">
+      <c r="D218" s="18">
         <v>2018</v>
       </c>
-      <c r="E218" s="21" t="s">
+      <c r="E218" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F218" s="21" t="s">
+      <c r="F218" s="18" t="s">
         <v>1717</v>
       </c>
-      <c r="G218" s="21" t="s">
+      <c r="G218" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="H218" s="21" t="s">
+      <c r="H218" s="18" t="s">
         <v>1767</v>
       </c>
     </row>
     <row r="219" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="22" t="s">
+      <c r="A219" s="19" t="s">
         <v>1768</v>
       </c>
-      <c r="B219" s="21" t="s">
+      <c r="B219" s="18" t="s">
         <v>1610</v>
       </c>
-      <c r="C219" s="21" t="s">
+      <c r="C219" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D219" s="21">
+      <c r="D219" s="18">
         <v>2013</v>
       </c>
-      <c r="E219" s="21" t="s">
+      <c r="E219" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F219" s="21" t="s">
+      <c r="F219" s="18" t="s">
         <v>1621</v>
       </c>
-      <c r="G219" s="21" t="s">
+      <c r="G219" s="18" t="s">
         <v>1742</v>
       </c>
-      <c r="H219" s="21" t="s">
+      <c r="H219" s="18" t="s">
         <v>1769</v>
       </c>
     </row>
     <row r="220" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="22" t="s">
+      <c r="A220" s="19" t="s">
         <v>1770</v>
       </c>
-      <c r="B220" s="21" t="s">
+      <c r="B220" s="18" t="s">
         <v>1771</v>
       </c>
-      <c r="C220" s="21" t="s">
+      <c r="C220" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D220" s="21">
+      <c r="D220" s="18">
         <v>2018</v>
       </c>
-      <c r="E220" s="21" t="s">
+      <c r="E220" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F220" s="21" t="s">
+      <c r="F220" s="18" t="s">
         <v>1772</v>
       </c>
-      <c r="G220" s="21" t="s">
+      <c r="G220" s="18" t="s">
         <v>1773</v>
       </c>
-      <c r="H220" s="21" t="s">
+      <c r="H220" s="18" t="s">
         <v>1774</v>
       </c>
     </row>
     <row r="221" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="22" t="s">
+      <c r="A221" s="19" t="s">
         <v>1775</v>
       </c>
-      <c r="B221" s="21" t="s">
+      <c r="B221" s="18" t="s">
         <v>1776</v>
       </c>
-      <c r="C221" s="21" t="s">
+      <c r="C221" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D221" s="21">
+      <c r="D221" s="18">
         <v>2014</v>
       </c>
-      <c r="E221" s="21" t="s">
+      <c r="E221" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F221" s="21" t="s">
+      <c r="F221" s="18" t="s">
         <v>1777</v>
       </c>
-      <c r="G221" s="21" t="s">
+      <c r="G221" s="18" t="s">
         <v>1778</v>
       </c>
-      <c r="H221" s="21" t="s">
+      <c r="H221" s="18" t="s">
         <v>1779</v>
       </c>
     </row>
     <row r="222" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="22" t="s">
+      <c r="A222" s="19" t="s">
         <v>1780</v>
       </c>
-      <c r="B222" s="21" t="s">
+      <c r="B222" s="18" t="s">
         <v>1781</v>
       </c>
-      <c r="C222" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="D222" s="21">
+      <c r="C222" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="D222" s="18">
         <v>2007</v>
       </c>
-      <c r="E222" s="21" t="s">
+      <c r="E222" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F222" s="21" t="s">
+      <c r="F222" s="18" t="s">
         <v>1404</v>
       </c>
-      <c r="G222" s="21" t="s">
+      <c r="G222" s="18" t="s">
         <v>1782</v>
       </c>
-      <c r="H222" s="21" t="s">
+      <c r="H222" s="18" t="s">
         <v>1783</v>
       </c>
     </row>
@@ -16667,22 +16670,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -17382,22 +17385,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -19279,28 +19282,28 @@
       <c r="O58" s="7"/>
     </row>
     <row r="59" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
+      <c r="A59" s="19" t="s">
         <v>1899</v>
       </c>
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="18" t="s">
         <v>1900</v>
       </c>
-      <c r="C59" s="21" t="s">
+      <c r="C59" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D59" s="21">
+      <c r="D59" s="18">
         <v>2006</v>
       </c>
-      <c r="E59" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F59" s="21" t="s">
+      <c r="E59" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="18" t="s">
         <v>1902</v>
       </c>
-      <c r="G59" s="21" t="s">
+      <c r="G59" s="18" t="s">
         <v>1903</v>
       </c>
-      <c r="H59" s="21" t="s">
+      <c r="H59" s="18" t="s">
         <v>1904</v>
       </c>
       <c r="I59" s="7"/>
@@ -19312,28 +19315,28 @@
       <c r="O59" s="7"/>
     </row>
     <row r="60" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
+      <c r="A60" s="19" t="s">
         <v>1905</v>
       </c>
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="18" t="s">
         <v>1906</v>
       </c>
-      <c r="C60" s="21" t="s">
+      <c r="C60" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D60" s="21">
+      <c r="D60" s="18">
         <v>2006</v>
       </c>
-      <c r="E60" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F60" s="21" t="s">
+      <c r="E60" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="18" t="s">
         <v>1907</v>
       </c>
-      <c r="G60" s="21" t="s">
+      <c r="G60" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="H60" s="21" t="s">
+      <c r="H60" s="18" t="s">
         <v>1908</v>
       </c>
       <c r="I60" s="7"/>
@@ -19345,28 +19348,28 @@
       <c r="O60" s="7"/>
     </row>
     <row r="61" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="22" t="s">
+      <c r="A61" s="19" t="s">
         <v>1909</v>
       </c>
-      <c r="B61" s="21" t="s">
+      <c r="B61" s="18" t="s">
         <v>1906</v>
       </c>
-      <c r="C61" s="21" t="s">
+      <c r="C61" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D61" s="21">
+      <c r="D61" s="18">
         <v>2011</v>
       </c>
-      <c r="E61" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F61" s="21" t="s">
+      <c r="E61" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="18" t="s">
         <v>1907</v>
       </c>
-      <c r="G61" s="21" t="s">
+      <c r="G61" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="H61" s="21" t="s">
+      <c r="H61" s="18" t="s">
         <v>1908</v>
       </c>
       <c r="I61" s="7"/>
@@ -19378,28 +19381,28 @@
       <c r="O61" s="7"/>
     </row>
     <row r="62" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
+      <c r="A62" s="19" t="s">
         <v>1910</v>
       </c>
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="18" t="s">
         <v>1911</v>
       </c>
-      <c r="C62" s="21" t="s">
+      <c r="C62" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D62" s="21">
+      <c r="D62" s="18">
         <v>2014</v>
       </c>
-      <c r="E62" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" s="21" t="s">
+      <c r="E62" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="18" t="s">
         <v>1912</v>
       </c>
-      <c r="G62" s="21" t="s">
+      <c r="G62" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="H62" s="21" t="s">
+      <c r="H62" s="18" t="s">
         <v>1913</v>
       </c>
       <c r="I62" s="7"/>
@@ -19411,28 +19414,28 @@
       <c r="O62" s="7"/>
     </row>
     <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="s">
+      <c r="A63" s="19" t="s">
         <v>1914</v>
       </c>
-      <c r="B63" s="21" t="s">
+      <c r="B63" s="18" t="s">
         <v>1915</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="C63" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D63" s="21">
+      <c r="D63" s="18">
         <v>2011</v>
       </c>
-      <c r="E63" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F63" s="21" t="s">
+      <c r="E63" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="18" t="s">
         <v>1916</v>
       </c>
-      <c r="G63" s="21" t="s">
+      <c r="G63" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="H63" s="21" t="s">
+      <c r="H63" s="18" t="s">
         <v>1917</v>
       </c>
       <c r="I63" s="7"/>
@@ -19444,28 +19447,28 @@
       <c r="O63" s="7"/>
     </row>
     <row r="64" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="19" t="s">
         <v>1918</v>
       </c>
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="18" t="s">
         <v>1919</v>
       </c>
-      <c r="C64" s="21" t="s">
+      <c r="C64" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D64" s="21">
+      <c r="D64" s="18">
         <v>2018</v>
       </c>
-      <c r="E64" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F64" s="21" t="s">
+      <c r="E64" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="18" t="s">
         <v>1920</v>
       </c>
-      <c r="G64" s="21" t="s">
+      <c r="G64" s="18" t="s">
         <v>1473</v>
       </c>
-      <c r="H64" s="21" t="s">
+      <c r="H64" s="18" t="s">
         <v>1921</v>
       </c>
       <c r="I64" s="7"/>
@@ -19516,22 +19519,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -19734,22 +19737,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -19825,22 +19828,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -19948,22 +19951,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -20010,7 +20013,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1003"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="G217" sqref="G217"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20047,22 +20052,22 @@
       <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -27127,7 +27132,7 @@
         <v>288</v>
       </c>
       <c r="G217" s="13" t="s">
-        <v>156</v>
+        <v>1931</v>
       </c>
       <c r="H217" s="7" t="s">
         <v>1005</v>
@@ -32698,28 +32703,28 @@
       <c r="O386" s="7"/>
     </row>
     <row r="387" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A387" s="22" t="s">
+      <c r="A387" s="19" t="s">
         <v>1899</v>
       </c>
-      <c r="B387" s="21" t="s">
+      <c r="B387" s="18" t="s">
         <v>1900</v>
       </c>
-      <c r="C387" s="21" t="s">
+      <c r="C387" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D387" s="21">
+      <c r="D387" s="18">
         <v>2006</v>
       </c>
-      <c r="E387" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F387" s="21" t="s">
+      <c r="E387" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F387" s="18" t="s">
         <v>1902</v>
       </c>
-      <c r="G387" s="21" t="s">
+      <c r="G387" s="18" t="s">
         <v>1903</v>
       </c>
-      <c r="H387" s="21" t="s">
+      <c r="H387" s="18" t="s">
         <v>1904</v>
       </c>
       <c r="I387" s="7"/>
@@ -32731,28 +32736,28 @@
       <c r="O387" s="7"/>
     </row>
     <row r="388" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A388" s="22" t="s">
+      <c r="A388" s="19" t="s">
         <v>1905</v>
       </c>
-      <c r="B388" s="21" t="s">
+      <c r="B388" s="18" t="s">
         <v>1906</v>
       </c>
-      <c r="C388" s="21" t="s">
+      <c r="C388" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D388" s="21">
+      <c r="D388" s="18">
         <v>2006</v>
       </c>
-      <c r="E388" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F388" s="21" t="s">
+      <c r="E388" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F388" s="18" t="s">
         <v>1907</v>
       </c>
-      <c r="G388" s="21" t="s">
+      <c r="G388" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="H388" s="21" t="s">
+      <c r="H388" s="18" t="s">
         <v>1908</v>
       </c>
       <c r="I388" s="7"/>
@@ -32764,28 +32769,28 @@
       <c r="O388" s="7"/>
     </row>
     <row r="389" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A389" s="22" t="s">
+      <c r="A389" s="19" t="s">
         <v>1909</v>
       </c>
-      <c r="B389" s="21" t="s">
+      <c r="B389" s="18" t="s">
         <v>1906</v>
       </c>
-      <c r="C389" s="21" t="s">
+      <c r="C389" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D389" s="21">
+      <c r="D389" s="18">
         <v>2011</v>
       </c>
-      <c r="E389" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F389" s="21" t="s">
+      <c r="E389" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F389" s="18" t="s">
         <v>1907</v>
       </c>
-      <c r="G389" s="21" t="s">
+      <c r="G389" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="H389" s="21" t="s">
+      <c r="H389" s="18" t="s">
         <v>1908</v>
       </c>
       <c r="I389" s="7"/>
@@ -32797,28 +32802,28 @@
       <c r="O389" s="7"/>
     </row>
     <row r="390" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A390" s="22" t="s">
+      <c r="A390" s="19" t="s">
         <v>1910</v>
       </c>
-      <c r="B390" s="21" t="s">
+      <c r="B390" s="18" t="s">
         <v>1911</v>
       </c>
-      <c r="C390" s="21" t="s">
+      <c r="C390" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D390" s="21">
+      <c r="D390" s="18">
         <v>2014</v>
       </c>
-      <c r="E390" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F390" s="21" t="s">
+      <c r="E390" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F390" s="18" t="s">
         <v>1912</v>
       </c>
-      <c r="G390" s="21" t="s">
+      <c r="G390" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="H390" s="21" t="s">
+      <c r="H390" s="18" t="s">
         <v>1913</v>
       </c>
       <c r="I390" s="7"/>
@@ -32830,28 +32835,28 @@
       <c r="O390" s="7"/>
     </row>
     <row r="391" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A391" s="22" t="s">
+      <c r="A391" s="19" t="s">
         <v>1914</v>
       </c>
-      <c r="B391" s="21" t="s">
+      <c r="B391" s="18" t="s">
         <v>1915</v>
       </c>
-      <c r="C391" s="21" t="s">
+      <c r="C391" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D391" s="21">
+      <c r="D391" s="18">
         <v>2011</v>
       </c>
-      <c r="E391" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F391" s="21" t="s">
+      <c r="E391" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F391" s="18" t="s">
         <v>1916</v>
       </c>
-      <c r="G391" s="21" t="s">
+      <c r="G391" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="H391" s="21" t="s">
+      <c r="H391" s="18" t="s">
         <v>1917</v>
       </c>
       <c r="I391" s="7"/>
@@ -32863,28 +32868,28 @@
       <c r="O391" s="7"/>
     </row>
     <row r="392" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A392" s="22" t="s">
+      <c r="A392" s="19" t="s">
         <v>1918</v>
       </c>
-      <c r="B392" s="21" t="s">
+      <c r="B392" s="18" t="s">
         <v>1919</v>
       </c>
-      <c r="C392" s="21" t="s">
+      <c r="C392" s="18" t="s">
         <v>1901</v>
       </c>
-      <c r="D392" s="21">
+      <c r="D392" s="18">
         <v>2018</v>
       </c>
-      <c r="E392" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F392" s="21" t="s">
+      <c r="E392" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F392" s="18" t="s">
         <v>1920</v>
       </c>
-      <c r="G392" s="21" t="s">
+      <c r="G392" s="18" t="s">
         <v>1473</v>
       </c>
-      <c r="H392" s="21" t="s">
+      <c r="H392" s="18" t="s">
         <v>1921</v>
       </c>
       <c r="I392" s="7"/>
@@ -32896,28 +32901,28 @@
       <c r="O392" s="7"/>
     </row>
     <row r="393" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A393" s="22" t="s">
+      <c r="A393" s="19" t="s">
         <v>1922</v>
       </c>
-      <c r="B393" s="21" t="s">
+      <c r="B393" s="18" t="s">
         <v>1923</v>
       </c>
-      <c r="C393" s="21" t="s">
+      <c r="C393" s="18" t="s">
         <v>833</v>
       </c>
-      <c r="D393" s="21">
+      <c r="D393" s="18">
         <v>2018</v>
       </c>
-      <c r="E393" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F393" s="21" t="s">
+      <c r="E393" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F393" s="18" t="s">
         <v>1924</v>
       </c>
-      <c r="G393" s="21" t="s">
+      <c r="G393" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="H393" s="21" t="s">
+      <c r="H393" s="18" t="s">
         <v>1925</v>
       </c>
       <c r="I393" s="7"/>
@@ -32929,28 +32934,28 @@
       <c r="O393" s="7"/>
     </row>
     <row r="394" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A394" s="22" t="s">
+      <c r="A394" s="19" t="s">
         <v>1926</v>
       </c>
-      <c r="B394" s="21" t="s">
+      <c r="B394" s="18" t="s">
         <v>1927</v>
       </c>
-      <c r="C394" s="21" t="s">
+      <c r="C394" s="18" t="s">
         <v>833</v>
       </c>
-      <c r="D394" s="21">
+      <c r="D394" s="18">
         <v>2008</v>
       </c>
-      <c r="E394" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F394" s="21" t="s">
+      <c r="E394" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F394" s="18" t="s">
         <v>1928</v>
       </c>
-      <c r="G394" s="21" t="s">
+      <c r="G394" s="18" t="s">
         <v>1929</v>
       </c>
-      <c r="H394" s="21" t="s">
+      <c r="H394" s="18" t="s">
         <v>1930</v>
       </c>
       <c r="I394" s="7"/>
@@ -32962,32 +32967,32 @@
       <c r="O394" s="7"/>
     </row>
     <row r="395" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A395" s="22" t="s">
+      <c r="A395" s="19" t="s">
         <v>1701</v>
       </c>
-      <c r="B395" s="21" t="s">
+      <c r="B395" s="18" t="s">
         <v>1702</v>
       </c>
-      <c r="C395" s="21" t="s">
+      <c r="C395" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D395" s="21">
+      <c r="D395" s="18">
         <v>2014</v>
       </c>
-      <c r="E395" s="21" t="s">
+      <c r="E395" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F395" s="21" t="s">
+      <c r="F395" s="18" t="s">
         <v>1703</v>
       </c>
-      <c r="G395" s="21" t="s">
+      <c r="G395" s="18" t="s">
         <v>1704</v>
       </c>
-      <c r="H395" s="21" t="s">
+      <c r="H395" s="18" t="s">
         <v>1705</v>
       </c>
-      <c r="I395" s="19"/>
-      <c r="J395" s="20"/>
+      <c r="I395" s="16"/>
+      <c r="J395" s="17"/>
       <c r="K395" s="7"/>
       <c r="L395" s="7"/>
       <c r="M395" s="7"/>
@@ -32995,32 +33000,32 @@
       <c r="O395" s="7"/>
     </row>
     <row r="396" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A396" s="22" t="s">
+      <c r="A396" s="19" t="s">
         <v>1706</v>
       </c>
-      <c r="B396" s="21" t="s">
+      <c r="B396" s="18" t="s">
         <v>1707</v>
       </c>
-      <c r="C396" s="21" t="s">
+      <c r="C396" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D396" s="21">
+      <c r="D396" s="18">
         <v>2018</v>
       </c>
-      <c r="E396" s="21" t="s">
+      <c r="E396" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F396" s="21" t="s">
+      <c r="F396" s="18" t="s">
         <v>1708</v>
       </c>
-      <c r="G396" s="21" t="s">
+      <c r="G396" s="18" t="s">
         <v>604</v>
       </c>
-      <c r="H396" s="21" t="s">
+      <c r="H396" s="18" t="s">
         <v>1709</v>
       </c>
-      <c r="I396" s="19"/>
-      <c r="J396" s="20"/>
+      <c r="I396" s="16"/>
+      <c r="J396" s="17"/>
       <c r="K396" s="7"/>
       <c r="L396" s="7"/>
       <c r="M396" s="7"/>
@@ -33028,32 +33033,32 @@
       <c r="O396" s="7"/>
     </row>
     <row r="397" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A397" s="22" t="s">
+      <c r="A397" s="19" t="s">
         <v>1710</v>
       </c>
-      <c r="B397" s="21" t="s">
+      <c r="B397" s="18" t="s">
         <v>1711</v>
       </c>
-      <c r="C397" s="21" t="s">
+      <c r="C397" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D397" s="21">
+      <c r="D397" s="18">
         <v>2018</v>
       </c>
-      <c r="E397" s="21" t="s">
+      <c r="E397" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F397" s="21" t="s">
+      <c r="F397" s="18" t="s">
         <v>1712</v>
       </c>
-      <c r="G397" s="21" t="s">
+      <c r="G397" s="18" t="s">
         <v>1713</v>
       </c>
-      <c r="H397" s="21" t="s">
+      <c r="H397" s="18" t="s">
         <v>1714</v>
       </c>
-      <c r="I397" s="19"/>
-      <c r="J397" s="20"/>
+      <c r="I397" s="16"/>
+      <c r="J397" s="17"/>
       <c r="K397" s="7"/>
       <c r="L397" s="7"/>
       <c r="M397" s="7"/>
@@ -33061,32 +33066,32 @@
       <c r="O397" s="7"/>
     </row>
     <row r="398" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A398" s="22" t="s">
+      <c r="A398" s="19" t="s">
         <v>1715</v>
       </c>
-      <c r="B398" s="21" t="s">
+      <c r="B398" s="18" t="s">
         <v>1716</v>
       </c>
-      <c r="C398" s="21" t="s">
+      <c r="C398" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D398" s="21">
+      <c r="D398" s="18">
         <v>2018</v>
       </c>
-      <c r="E398" s="21" t="s">
+      <c r="E398" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F398" s="21" t="s">
+      <c r="F398" s="18" t="s">
         <v>1717</v>
       </c>
-      <c r="G398" s="21" t="s">
+      <c r="G398" s="18" t="s">
         <v>1718</v>
       </c>
-      <c r="H398" s="21" t="s">
+      <c r="H398" s="18" t="s">
         <v>1719</v>
       </c>
-      <c r="I398" s="19"/>
-      <c r="J398" s="20"/>
+      <c r="I398" s="16"/>
+      <c r="J398" s="17"/>
       <c r="K398" s="7"/>
       <c r="L398" s="7"/>
       <c r="M398" s="7"/>
@@ -33094,32 +33099,32 @@
       <c r="O398" s="7"/>
     </row>
     <row r="399" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A399" s="22" t="s">
+      <c r="A399" s="19" t="s">
         <v>1720</v>
       </c>
-      <c r="B399" s="21" t="s">
+      <c r="B399" s="18" t="s">
         <v>1721</v>
       </c>
-      <c r="C399" s="21" t="s">
+      <c r="C399" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D399" s="21">
+      <c r="D399" s="18">
         <v>2018</v>
       </c>
-      <c r="E399" s="21" t="s">
+      <c r="E399" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F399" s="21" t="s">
+      <c r="F399" s="18" t="s">
         <v>1722</v>
       </c>
-      <c r="G399" s="21" t="s">
+      <c r="G399" s="18" t="s">
         <v>1723</v>
       </c>
-      <c r="H399" s="21" t="s">
+      <c r="H399" s="18" t="s">
         <v>1724</v>
       </c>
-      <c r="I399" s="19"/>
-      <c r="J399" s="20"/>
+      <c r="I399" s="16"/>
+      <c r="J399" s="17"/>
       <c r="K399" s="7"/>
       <c r="L399" s="7"/>
       <c r="M399" s="7"/>
@@ -33127,32 +33132,32 @@
       <c r="O399" s="7"/>
     </row>
     <row r="400" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A400" s="22" t="s">
+      <c r="A400" s="19" t="s">
         <v>1725</v>
       </c>
-      <c r="B400" s="21" t="s">
+      <c r="B400" s="18" t="s">
         <v>1726</v>
       </c>
-      <c r="C400" s="21" t="s">
+      <c r="C400" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D400" s="21">
+      <c r="D400" s="18">
         <v>2018</v>
       </c>
-      <c r="E400" s="21" t="s">
+      <c r="E400" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F400" s="21" t="s">
+      <c r="F400" s="18" t="s">
         <v>1727</v>
       </c>
-      <c r="G400" s="21" t="s">
+      <c r="G400" s="18" t="s">
         <v>1728</v>
       </c>
-      <c r="H400" s="21" t="s">
+      <c r="H400" s="18" t="s">
         <v>1729</v>
       </c>
-      <c r="I400" s="19"/>
-      <c r="J400" s="20"/>
+      <c r="I400" s="16"/>
+      <c r="J400" s="17"/>
       <c r="K400" s="7"/>
       <c r="L400" s="7"/>
       <c r="M400" s="7"/>
@@ -33160,32 +33165,32 @@
       <c r="O400" s="7"/>
     </row>
     <row r="401" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A401" s="22" t="s">
+      <c r="A401" s="19" t="s">
         <v>1730</v>
       </c>
-      <c r="B401" s="21" t="s">
+      <c r="B401" s="18" t="s">
         <v>1731</v>
       </c>
-      <c r="C401" s="21" t="s">
+      <c r="C401" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D401" s="21">
+      <c r="D401" s="18">
         <v>2018</v>
       </c>
-      <c r="E401" s="21" t="s">
+      <c r="E401" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F401" s="21" t="s">
+      <c r="F401" s="18" t="s">
         <v>1732</v>
       </c>
-      <c r="G401" s="21" t="s">
+      <c r="G401" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="H401" s="21" t="s">
+      <c r="H401" s="18" t="s">
         <v>1733</v>
       </c>
-      <c r="I401" s="19"/>
-      <c r="J401" s="20"/>
+      <c r="I401" s="16"/>
+      <c r="J401" s="17"/>
       <c r="K401" s="7"/>
       <c r="L401" s="7"/>
       <c r="M401" s="7"/>
@@ -33193,28 +33198,28 @@
       <c r="O401" s="7"/>
     </row>
     <row r="402" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A402" s="22" t="s">
+      <c r="A402" s="19" t="s">
         <v>1734</v>
       </c>
-      <c r="B402" s="21" t="s">
+      <c r="B402" s="18" t="s">
         <v>1735</v>
       </c>
-      <c r="C402" s="21" t="s">
+      <c r="C402" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D402" s="21">
+      <c r="D402" s="18">
         <v>2011</v>
       </c>
-      <c r="E402" s="21" t="s">
+      <c r="E402" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F402" s="21" t="s">
+      <c r="F402" s="18" t="s">
         <v>1736</v>
       </c>
-      <c r="G402" s="21" t="s">
+      <c r="G402" s="18" t="s">
         <v>1737</v>
       </c>
-      <c r="H402" s="21" t="s">
+      <c r="H402" s="18" t="s">
         <v>1738</v>
       </c>
       <c r="I402" s="7"/>
@@ -33226,28 +33231,28 @@
       <c r="O402" s="7"/>
     </row>
     <row r="403" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A403" s="22" t="s">
+      <c r="A403" s="19" t="s">
         <v>1739</v>
       </c>
-      <c r="B403" s="21" t="s">
+      <c r="B403" s="18" t="s">
         <v>1740</v>
       </c>
-      <c r="C403" s="21" t="s">
+      <c r="C403" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D403" s="21">
+      <c r="D403" s="18">
         <v>2015</v>
       </c>
-      <c r="E403" s="21" t="s">
+      <c r="E403" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F403" s="21" t="s">
+      <c r="F403" s="18" t="s">
         <v>1741</v>
       </c>
-      <c r="G403" s="21" t="s">
+      <c r="G403" s="18" t="s">
         <v>1742</v>
       </c>
-      <c r="H403" s="21" t="s">
+      <c r="H403" s="18" t="s">
         <v>1743</v>
       </c>
       <c r="I403" s="7"/>
@@ -33259,28 +33264,28 @@
       <c r="O403" s="7"/>
     </row>
     <row r="404" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A404" s="22" t="s">
+      <c r="A404" s="19" t="s">
         <v>1744</v>
       </c>
-      <c r="B404" s="21" t="s">
+      <c r="B404" s="18" t="s">
         <v>1745</v>
       </c>
-      <c r="C404" s="21" t="s">
+      <c r="C404" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D404" s="21">
+      <c r="D404" s="18">
         <v>2018</v>
       </c>
-      <c r="E404" s="21" t="s">
+      <c r="E404" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F404" s="21" t="s">
+      <c r="F404" s="18" t="s">
         <v>1746</v>
       </c>
-      <c r="G404" s="21" t="s">
+      <c r="G404" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="H404" s="21" t="s">
+      <c r="H404" s="18" t="s">
         <v>1747</v>
       </c>
       <c r="I404" s="7"/>
@@ -33292,28 +33297,28 @@
       <c r="O404" s="7"/>
     </row>
     <row r="405" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A405" s="22" t="s">
+      <c r="A405" s="19" t="s">
         <v>1748</v>
       </c>
-      <c r="B405" s="21" t="s">
+      <c r="B405" s="18" t="s">
         <v>1749</v>
       </c>
-      <c r="C405" s="21" t="s">
+      <c r="C405" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D405" s="21">
+      <c r="D405" s="18">
         <v>2015</v>
       </c>
-      <c r="E405" s="21" t="s">
+      <c r="E405" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F405" s="21" t="s">
+      <c r="F405" s="18" t="s">
         <v>1750</v>
       </c>
-      <c r="G405" s="21" t="s">
+      <c r="G405" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="H405" s="21" t="s">
+      <c r="H405" s="18" t="s">
         <v>1751</v>
       </c>
       <c r="I405" s="7"/>
@@ -33325,28 +33330,28 @@
       <c r="O405" s="7"/>
     </row>
     <row r="406" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A406" s="22" t="s">
+      <c r="A406" s="19" t="s">
         <v>1752</v>
       </c>
-      <c r="B406" s="21" t="s">
+      <c r="B406" s="18" t="s">
         <v>1753</v>
       </c>
-      <c r="C406" s="21" t="s">
+      <c r="C406" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D406" s="21">
+      <c r="D406" s="18">
         <v>2018</v>
       </c>
-      <c r="E406" s="21" t="s">
+      <c r="E406" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F406" s="21" t="s">
+      <c r="F406" s="18" t="s">
         <v>1754</v>
       </c>
-      <c r="G406" s="21" t="s">
+      <c r="G406" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="H406" s="21" t="s">
+      <c r="H406" s="18" t="s">
         <v>1755</v>
       </c>
       <c r="I406" s="7"/>
@@ -33358,28 +33363,28 @@
       <c r="O406" s="7"/>
     </row>
     <row r="407" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A407" s="22" t="s">
+      <c r="A407" s="19" t="s">
         <v>1756</v>
       </c>
-      <c r="B407" s="21" t="s">
+      <c r="B407" s="18" t="s">
         <v>1757</v>
       </c>
-      <c r="C407" s="21" t="s">
+      <c r="C407" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D407" s="21">
+      <c r="D407" s="18">
         <v>2018</v>
       </c>
-      <c r="E407" s="21" t="s">
+      <c r="E407" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F407" s="21" t="s">
+      <c r="F407" s="18" t="s">
         <v>1758</v>
       </c>
-      <c r="G407" s="21" t="s">
+      <c r="G407" s="18" t="s">
         <v>1759</v>
       </c>
-      <c r="H407" s="21" t="s">
+      <c r="H407" s="18" t="s">
         <v>1760</v>
       </c>
       <c r="I407" s="7"/>
@@ -33391,158 +33396,158 @@
       <c r="O407" s="7"/>
     </row>
     <row r="408" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A408" s="22" t="s">
+      <c r="A408" s="19" t="s">
         <v>1761</v>
       </c>
-      <c r="B408" s="21" t="s">
+      <c r="B408" s="18" t="s">
         <v>1762</v>
       </c>
-      <c r="C408" s="21" t="s">
+      <c r="C408" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D408" s="21">
+      <c r="D408" s="18">
         <v>2010</v>
       </c>
-      <c r="E408" s="21" t="s">
+      <c r="E408" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F408" s="21" t="s">
+      <c r="F408" s="18" t="s">
         <v>1763</v>
       </c>
-      <c r="G408" s="21" t="s">
+      <c r="G408" s="18" t="s">
         <v>1645</v>
       </c>
-      <c r="H408" s="21" t="s">
+      <c r="H408" s="18" t="s">
         <v>1764</v>
       </c>
     </row>
     <row r="409" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A409" s="22" t="s">
+      <c r="A409" s="19" t="s">
         <v>1765</v>
       </c>
-      <c r="B409" s="21" t="s">
+      <c r="B409" s="18" t="s">
         <v>1766</v>
       </c>
-      <c r="C409" s="21" t="s">
+      <c r="C409" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D409" s="21">
+      <c r="D409" s="18">
         <v>2018</v>
       </c>
-      <c r="E409" s="21" t="s">
+      <c r="E409" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F409" s="21" t="s">
+      <c r="F409" s="18" t="s">
         <v>1717</v>
       </c>
-      <c r="G409" s="21" t="s">
+      <c r="G409" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="H409" s="21" t="s">
+      <c r="H409" s="18" t="s">
         <v>1767</v>
       </c>
     </row>
     <row r="410" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="19" t="s">
         <v>1768</v>
       </c>
-      <c r="B410" s="21" t="s">
+      <c r="B410" s="18" t="s">
         <v>1610</v>
       </c>
-      <c r="C410" s="21" t="s">
+      <c r="C410" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D410" s="21">
+      <c r="D410" s="18">
         <v>2013</v>
       </c>
-      <c r="E410" s="21" t="s">
+      <c r="E410" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F410" s="21" t="s">
+      <c r="F410" s="18" t="s">
         <v>1621</v>
       </c>
-      <c r="G410" s="21" t="s">
+      <c r="G410" s="18" t="s">
         <v>1742</v>
       </c>
-      <c r="H410" s="21" t="s">
+      <c r="H410" s="18" t="s">
         <v>1769</v>
       </c>
     </row>
     <row r="411" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A411" s="22" t="s">
+      <c r="A411" s="19" t="s">
         <v>1770</v>
       </c>
-      <c r="B411" s="21" t="s">
+      <c r="B411" s="18" t="s">
         <v>1771</v>
       </c>
-      <c r="C411" s="21" t="s">
+      <c r="C411" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D411" s="21">
+      <c r="D411" s="18">
         <v>2018</v>
       </c>
-      <c r="E411" s="21" t="s">
+      <c r="E411" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F411" s="21" t="s">
+      <c r="F411" s="18" t="s">
         <v>1772</v>
       </c>
-      <c r="G411" s="21" t="s">
+      <c r="G411" s="18" t="s">
         <v>1773</v>
       </c>
-      <c r="H411" s="21" t="s">
+      <c r="H411" s="18" t="s">
         <v>1774</v>
       </c>
     </row>
     <row r="412" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A412" s="22" t="s">
+      <c r="A412" s="19" t="s">
         <v>1775</v>
       </c>
-      <c r="B412" s="21" t="s">
+      <c r="B412" s="18" t="s">
         <v>1776</v>
       </c>
-      <c r="C412" s="21" t="s">
+      <c r="C412" s="18" t="s">
         <v>1408</v>
       </c>
-      <c r="D412" s="21">
+      <c r="D412" s="18">
         <v>2014</v>
       </c>
-      <c r="E412" s="21" t="s">
+      <c r="E412" s="18" t="s">
         <v>1409</v>
       </c>
-      <c r="F412" s="21" t="s">
+      <c r="F412" s="18" t="s">
         <v>1777</v>
       </c>
-      <c r="G412" s="21" t="s">
+      <c r="G412" s="18" t="s">
         <v>1778</v>
       </c>
-      <c r="H412" s="21" t="s">
+      <c r="H412" s="18" t="s">
         <v>1779</v>
       </c>
     </row>
     <row r="413" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A413" s="22" t="s">
+      <c r="A413" s="19" t="s">
         <v>1780</v>
       </c>
-      <c r="B413" s="21" t="s">
+      <c r="B413" s="18" t="s">
         <v>1781</v>
       </c>
-      <c r="C413" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="D413" s="21">
+      <c r="C413" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="D413" s="18">
         <v>2007</v>
       </c>
-      <c r="E413" s="21" t="s">
+      <c r="E413" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F413" s="21" t="s">
+      <c r="F413" s="18" t="s">
         <v>1404</v>
       </c>
-      <c r="G413" s="21" t="s">
+      <c r="G413" s="18" t="s">
         <v>1782</v>
       </c>
-      <c r="H413" s="21" t="s">
+      <c r="H413" s="18" t="s">
         <v>1783</v>
       </c>
     </row>
@@ -34197,22 +34202,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -34636,22 +34641,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -34763,22 +34768,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -35247,22 +35252,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -35397,28 +35402,28 @@
       <c r="O5" s="7"/>
     </row>
     <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="19" t="s">
         <v>1922</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="18" t="s">
         <v>1923</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="18" t="s">
         <v>833</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="18">
         <v>2018</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="21" t="s">
+      <c r="E6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>1924</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="18" t="s">
         <v>1925</v>
       </c>
       <c r="I6" s="7"/>
@@ -35430,28 +35435,28 @@
       <c r="O6" s="7"/>
     </row>
     <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>1926</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="18" t="s">
         <v>1927</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="18" t="s">
         <v>833</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="18">
         <v>2008</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="21" t="s">
+      <c r="E7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>1928</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="18" t="s">
         <v>1929</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="18" t="s">
         <v>1930</v>
       </c>
       <c r="I7" s="7"/>
@@ -35475,7 +35480,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:U7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -35502,22 +35507,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="25.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -35700,7 +35705,7 @@
         <v>288</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>156</v>
+        <v>1931</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>1005</v>
@@ -35753,22 +35758,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -36163,22 +36168,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -36715,22 +36720,22 @@
       <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="18"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
BRS 14 to tr excel
</commit_message>
<xml_diff>
--- a/downloads/trlist.xlsx
+++ b/downloads/trlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="3" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARS" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5874" uniqueCount="1954">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5875" uniqueCount="1955">
   <si>
     <t>NO</t>
   </si>
@@ -8260,6 +8260,9 @@
   </si>
   <si>
     <t>Başkent Üniversitesi Kadın- Çocuk Sağlığı ve Aile Planlaması Araştırma ve Uygulama Merkezi (BÜKÇAM) ve UNFPA ortaklığıyla ve Sabancı Vakfı destekleriyle 2019 yılında gerçekleştirilen “Çocuk Yaşta Evliliklerin Önlenmesi Projesi: Nevşehir Modeli” çalışması kapsamında geliştirilen bu broşürler hem çocuk yaşta evliliklerin sağlık sonuçlarına hem de çocuk, ergen, genç ve yetişkin kayramlarına odaklanıyor.</t>
+  </si>
+  <si>
+    <t>BRS_14</t>
   </si>
 </sst>
 </file>
@@ -20096,7 +20099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+    <sheetView topLeftCell="A184" workbookViewId="0">
       <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
@@ -34410,10 +34413,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -34873,6 +34876,11 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>1954</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>